<commit_message>
updated test values to reflect excel properly
</commit_message>
<xml_diff>
--- a/casos de prueba Codidgo_limpio1.0.xlsx
+++ b/casos de prueba Codidgo_limpio1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b12s307\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63D19B0-9061-406B-B758-6AA88A07D5AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E716AE-718F-448C-8221-48EBBC05E63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>Fecha de fin</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Sueldo</t>
   </si>
   <si>
-    <t>Motivo del Retiro</t>
-  </si>
-  <si>
     <t>Renuncia Voluntaria</t>
   </si>
   <si>
@@ -141,14 +138,18 @@
   </si>
   <si>
     <t>dias indemnización</t>
+  </si>
+  <si>
+    <t>Sueldo + auxilio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -193,7 +194,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +216,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -245,9 +252,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -270,7 +277,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -285,9 +292,15 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -620,18 +633,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B6:L23"/>
+  <dimension ref="B6:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="1"/>
     <col min="2" max="2" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="26.140625" style="1" bestFit="1" customWidth="1"/>
@@ -672,69 +686,69 @@
     </row>
     <row r="7" spans="2:12" ht="24" x14ac:dyDescent="0.25">
       <c r="C7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="G7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="H7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="I7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="J7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="K7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>7</v>
-      </c>
       <c r="L7" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="42" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>10</v>
-      </c>
       <c r="E8" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F8" s="3">
         <v>44197</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I8" s="3">
         <v>44197</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="21" x14ac:dyDescent="0.25">
@@ -742,25 +756,25 @@
         <v>0</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="G9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H9" s="3">
         <v>45597</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J9" s="3">
         <v>45302</v>
@@ -774,34 +788,34 @@
     </row>
     <row r="10" spans="2:12" ht="21" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="8">
+        <v>1462000</v>
+      </c>
+      <c r="D10" s="8">
+        <v>1662000</v>
+      </c>
+      <c r="E10" s="8">
+        <v>3662000</v>
+      </c>
+      <c r="F10" s="8">
+        <v>1462000</v>
+      </c>
+      <c r="G10" s="8">
+        <v>1462000</v>
+      </c>
+      <c r="H10" s="8">
+        <v>1600000</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="L10" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -841,7 +855,7 @@
     </row>
     <row r="12" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="1">
         <v>0</v>
@@ -862,21 +876,21 @@
         <v>0</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="1">
         <v>0</v>
@@ -897,21 +911,21 @@
         <v>0</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K13" s="1">
         <v>31</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="s">
-        <v>34</v>
+      <c r="B14" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="C14" s="1">
         <v>0</v>
@@ -934,25 +948,25 @@
     </row>
     <row r="15" spans="2:12" ht="21" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="8">
         <v>609167</v>
       </c>
       <c r="D15" s="8">
-        <v>784333</v>
+        <v>1634300</v>
       </c>
       <c r="E15" s="8">
-        <v>1223445</v>
+        <v>1230839</v>
       </c>
       <c r="F15" s="8">
-        <v>2600000</v>
+        <v>6127800</v>
       </c>
       <c r="G15" s="8">
-        <v>678206</v>
+        <v>1360472</v>
       </c>
       <c r="H15" s="8">
-        <v>865015</v>
+        <v>1732633</v>
       </c>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
@@ -961,25 +975,25 @@
     </row>
     <row r="16" spans="2:12" ht="21" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="8">
         <v>270833</v>
       </c>
       <c r="D16" s="8">
-        <v>729167</v>
+        <v>737500</v>
       </c>
       <c r="E16" s="8">
-        <v>583333</v>
+        <v>588194</v>
       </c>
       <c r="F16" s="8">
-        <v>2600000</v>
+        <v>2634306</v>
       </c>
       <c r="G16" s="8">
-        <v>597639</v>
+        <v>604861</v>
       </c>
       <c r="H16" s="8">
-        <v>695833</v>
+        <v>786667</v>
       </c>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
@@ -988,25 +1002,25 @@
     </row>
     <row r="17" spans="2:12" ht="21" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="8">
         <v>609167</v>
       </c>
       <c r="D17" s="8">
-        <v>1615833</v>
+        <v>1634300</v>
       </c>
       <c r="E17" s="8">
-        <v>1222048</v>
+        <v>1230839</v>
       </c>
       <c r="F17" s="8">
-        <v>5200000</v>
+        <v>6127800</v>
       </c>
       <c r="G17" s="8">
-        <v>1396756</v>
+        <v>1360472</v>
       </c>
       <c r="H17" s="8">
-        <v>1622961</v>
+        <v>1732633</v>
       </c>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
@@ -1015,25 +1029,25 @@
     </row>
     <row r="18" spans="2:12" ht="21" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="8">
         <v>30458</v>
       </c>
       <c r="D18" s="8">
-        <v>188514</v>
+        <v>192847</v>
       </c>
       <c r="E18" s="8">
-        <v>48882</v>
+        <v>49644</v>
       </c>
       <c r="F18" s="8">
-        <v>624000</v>
+        <v>2980153</v>
       </c>
       <c r="G18" s="8">
-        <v>154109</v>
+        <v>151919</v>
       </c>
       <c r="H18" s="8">
-        <v>162837</v>
+        <v>204451</v>
       </c>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
@@ -1042,43 +1056,53 @@
     </row>
     <row r="19" spans="2:12" ht="42" x14ac:dyDescent="0.25">
       <c r="B19" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="8">
         <v>1519625</v>
       </c>
       <c r="D19" s="8">
-        <v>3585347</v>
+        <v>4198947</v>
       </c>
       <c r="E19" s="8">
-        <v>3077708</v>
+        <v>3099516</v>
       </c>
       <c r="F19" s="8">
-        <v>14924000</v>
+        <v>17870059</v>
       </c>
       <c r="G19" s="8">
-        <v>2420104</v>
+        <v>3477724</v>
       </c>
       <c r="H19" s="8">
-        <v>3397114</v>
+        <v>7123051</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="2:12" ht="21" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:12" ht="21" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:12" ht="21" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:12" ht="21" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="E21" s="8"/>
+      <c r="F21" s="14"/>
+    </row>
+    <row r="22" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E24" s="8"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>